<commit_message>
adding api template for the project in Vy_tempo
</commit_message>
<xml_diff>
--- a/Excel Tables/Known Species.xlsx
+++ b/Excel Tables/Known Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nugen\Desktop\DATA ANALYTICS COURSE\Project 3 (Module 16)\Project3_Group4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a735376cfa3b3e71/DataAnalyticsBootcamp2023/CourseModules/Assignment/Project3_Group4/Excel Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CA72E60-6137-4D86-896C-79B59B78103E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{2CA72E60-6137-4D86-896C-79B59B78103E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFAFB679-F5E4-4EBF-8544-30E92DD61B21}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11626" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OECD.Stat export" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>MyOECD</author>
   </authors>
   <commentList>
-    <comment ref="N29" authorId="0" shapeId="0">
+    <comment ref="N29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -250,9 +250,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -879,50 +879,8 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -930,23 +888,11 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -956,6 +902,60 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1311,18 +1311,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="26.1796875" customWidth="1"/>
-    <col min="3" max="3" width="2.36328125" customWidth="1"/>
+    <col min="1" max="2" width="26.17578125" customWidth="1"/>
+    <col min="3" max="3" width="2.3515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="e">
         <f ca="1">DotStatQuery(B1)</f>
         <v>#NAME?</v>
@@ -1331,1714 +1331,1739 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="22.7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="10"/>
-    </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.4">
+      <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="28"/>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="22">
+      <c r="B7" s="12"/>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6">
         <v>377</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="6">
         <v>798</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="6">
         <v>1085</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="6">
         <v>239</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="6">
         <v>5342</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="6">
         <v>5058</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="6">
         <v>315</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="6">
         <v>22949</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="6">
         <v>2020</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="6">
         <v>3880</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="6">
         <v>114940</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="23">
+      <c r="B8" s="12"/>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7">
         <v>104</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="7">
         <v>229</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="7">
         <v>14</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="7">
         <v>21</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="7">
         <v>99</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="23">
+      <c r="I8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="7">
         <v>99</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="7">
         <v>3054</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="7">
         <v>1016</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="7">
         <v>2100</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="7">
         <v>53464</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="22">
+      <c r="B9" s="12"/>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6">
         <v>84</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="6">
         <v>198</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="6">
         <v>10</v>
       </c>
-      <c r="G9" s="22">
-        <v>19</v>
-      </c>
-      <c r="H9" s="22">
+      <c r="G9" s="6">
+        <v>19</v>
+      </c>
+      <c r="H9" s="6">
         <v>142</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="6">
         <v>99</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="6">
         <v>43</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="6">
         <v>1818</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="6">
         <v>521</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="6">
         <v>838</v>
       </c>
-      <c r="N9" s="22">
+      <c r="N9" s="6">
         <v>5238</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="23">
+      <c r="B10" s="12"/>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7">
         <v>222</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="7">
         <v>691</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="7">
         <v>45</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="7">
         <v>46</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="7">
         <v>1392</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="7">
         <v>1229</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="7">
         <v>163</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="7">
         <v>5304</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="7">
         <v>1405</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="7">
         <v>2677</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="7">
         <v>31471</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="22">
+      <c r="B11" s="12"/>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6">
         <v>185</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="6">
         <v>510</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="6">
         <v>140</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="6">
         <v>65</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="6">
         <v>1272</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="6">
         <v>1182</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="6">
         <v>72</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="6">
         <v>6103</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="6">
         <v>923</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="6">
         <v>1383</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="6">
         <v>12220</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="23">
+      <c r="B12" s="12"/>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="7">
         <v>543</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="7">
         <v>1954</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="7">
         <v>638</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="7">
         <v>871</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="7">
         <v>4216</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="7">
         <v>2600</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="7">
         <v>1603</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="7">
         <v>38140</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="7">
         <v>1640</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="7">
         <v>1761</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="7">
         <v>22745</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="22">
+      <c r="B13" s="12"/>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="6">
         <v>241</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="6">
         <v>890</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="6">
         <v>196</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="6">
         <v>191</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="6">
         <v>2012</v>
       </c>
-      <c r="I13" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="22">
+      <c r="I13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="6">
         <v>1943</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="6">
         <v>4</v>
       </c>
-      <c r="M13" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="22">
+      <c r="M13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="6">
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="23">
+      <c r="B14" s="12"/>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="7">
         <v>92</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="7">
         <v>221</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="7">
         <v>13</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="7">
         <v>21</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="7">
         <v>80</v>
       </c>
-      <c r="I14" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="23">
+      <c r="I14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="7">
         <v>80</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="7">
         <v>2256</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="7">
         <v>886</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="7">
         <v>1526</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="7">
         <v>32000</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="22">
+      <c r="B15" s="12"/>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="6">
         <v>71</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="6">
         <v>241</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="6">
         <v>8</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="6">
         <v>15</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="6">
         <v>238</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="22">
+      <c r="I15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="6">
         <v>55</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="6">
         <v>2918</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="6">
         <v>452</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="6">
         <v>1002</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="6">
         <v>4270</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="23">
+      <c r="B16" s="12"/>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="7">
         <v>66</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="7">
         <v>234</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="7">
         <v>5</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="7">
         <v>11</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="7">
         <v>103</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="7">
         <v>66</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="7">
         <v>54</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="7">
         <v>2013</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="7">
         <v>598</v>
       </c>
-      <c r="M16" s="23">
+      <c r="M16" s="7">
         <v>556</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="7">
         <v>10371</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+    <row r="17" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="22">
+      <c r="B17" s="12"/>
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="6">
         <v>71</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="6">
         <v>253</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="6">
         <v>6</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="6">
         <v>10</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="6">
         <v>88</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="6">
         <v>25</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="6">
         <v>63</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="6">
         <v>2628</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="6">
         <v>929</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="6">
         <v>1898</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="6">
         <v>14647</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="23">
+      <c r="B18" s="12"/>
+      <c r="C18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="7">
         <v>125</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="7">
         <v>396</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="7">
         <v>38</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="7">
         <v>35</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="7">
         <v>163</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="7">
         <v>83</v>
       </c>
-      <c r="J18" s="23">
+      <c r="J18" s="7">
         <v>80</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="7">
         <v>4982</v>
       </c>
-      <c r="L18" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="23">
+      <c r="L18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="7">
         <v>1060</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+    <row r="19" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="22">
+      <c r="B19" s="14"/>
+      <c r="C19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="6">
         <v>107</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="6">
         <v>280</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="6">
         <v>13</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="6">
         <v>21</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="6">
         <v>197</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="6">
         <v>94</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="6">
         <v>103</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="6">
         <v>4305</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="6">
         <v>1195</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="6">
         <v>2380</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="6">
         <v>10434</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="23">
+      <c r="B20" s="12"/>
+      <c r="C20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="7">
         <v>115</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="7">
         <v>440</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="7">
         <v>66</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="7">
         <v>23</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="7">
         <v>665</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="7">
         <v>511</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J20" s="7">
         <v>154</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="7">
         <v>5850</v>
       </c>
-      <c r="L20" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="M20" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="N20" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+      <c r="L20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="22">
+      <c r="B21" s="12"/>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="6">
         <v>87</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="6">
         <v>238</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="6">
         <v>15</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="6">
         <v>18</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="6">
         <v>81</v>
       </c>
-      <c r="I21" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="22">
+      <c r="I21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="6">
         <v>81</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="6">
         <v>2721</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="6">
         <v>659</v>
       </c>
-      <c r="M21" s="22">
+      <c r="M21" s="6">
         <v>715</v>
       </c>
-      <c r="N21" s="22">
+      <c r="N21" s="6">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A22" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="23">
+      <c r="B22" s="12"/>
+      <c r="C22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="7">
         <v>4</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="7">
         <v>75</v>
       </c>
-      <c r="F22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="23">
+      <c r="F22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="7">
         <v>5</v>
       </c>
-      <c r="I22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="23">
+      <c r="I22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="7">
         <v>5</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="7">
         <v>438</v>
       </c>
-      <c r="L22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="N22" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="L22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A23" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="22">
+      <c r="B23" s="12"/>
+      <c r="C23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="6">
         <v>57</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="6">
         <v>489</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="6">
         <v>3</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="6">
         <v>3</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="6">
         <v>404</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="6">
         <v>376</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J23" s="6">
         <v>28</v>
       </c>
-      <c r="K23" s="22">
+      <c r="K23" s="6">
         <v>1050</v>
       </c>
-      <c r="L23" s="22">
+      <c r="L23" s="6">
         <v>596</v>
       </c>
-      <c r="M23" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N23" s="22">
+      <c r="M23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="6">
         <v>1230</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A24" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="23">
+      <c r="B24" s="12"/>
+      <c r="C24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="7">
         <v>126</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="7">
         <v>278</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="7">
         <v>56</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="7">
         <v>44</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="7">
         <v>641</v>
       </c>
-      <c r="I24" s="23">
+      <c r="I24" s="7">
         <v>544</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="7">
         <v>97</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="7">
         <v>8249</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="7">
         <v>1209</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="7">
         <v>2704</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="7">
         <v>58632</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A25" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="22">
+      <c r="B25" s="12"/>
+      <c r="C25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="6">
         <v>160</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="6">
         <v>700</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="6">
         <v>100</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="6">
         <v>91</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="6">
         <v>4300</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="6">
         <v>3900</v>
       </c>
-      <c r="J25" s="22">
+      <c r="J25" s="6">
         <v>400</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="6">
         <v>7000</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="6">
         <v>1800</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="6">
         <v>1600</v>
       </c>
-      <c r="N25" s="22">
+      <c r="N25" s="6">
         <v>5300</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A26" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="23">
+      <c r="B26" s="12"/>
+      <c r="C26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="7">
         <v>125</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="7">
         <v>548</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="7">
         <v>32</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="7">
         <v>27</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="7">
         <v>1326</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="7">
         <v>1102</v>
       </c>
-      <c r="J26" s="23">
+      <c r="J26" s="7">
         <v>224</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="7">
         <v>4606</v>
       </c>
-      <c r="L26" s="23">
+      <c r="L26" s="7">
         <v>1051</v>
       </c>
-      <c r="M26" s="23">
+      <c r="M26" s="7">
         <v>1133</v>
       </c>
-      <c r="N26" s="23">
+      <c r="N26" s="7">
         <v>30054</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+    <row r="27" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A27" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="22">
+      <c r="B27" s="12"/>
+      <c r="C27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="6">
         <v>62</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="6">
         <v>233</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="6">
         <v>7</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="6">
         <v>13</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="6">
         <v>87</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="6">
         <v>42</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J27" s="6">
         <v>45</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="6">
         <v>1937</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="6">
         <v>560</v>
       </c>
-      <c r="M27" s="22">
+      <c r="M27" s="6">
         <v>687</v>
       </c>
-      <c r="N27" s="22">
+      <c r="N27" s="6">
         <v>17100</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A28" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="23">
+      <c r="B28" s="12"/>
+      <c r="C28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="7">
         <v>68</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="7">
         <v>389</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="7">
         <v>7</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="7">
         <v>13</v>
       </c>
-      <c r="H28" s="23">
+      <c r="H28" s="7">
         <v>105</v>
       </c>
-      <c r="I28" s="23">
+      <c r="I28" s="7">
         <v>51</v>
       </c>
-      <c r="J28" s="23">
+      <c r="J28" s="7">
         <v>54</v>
       </c>
-      <c r="K28" s="23">
+      <c r="K28" s="7">
         <v>1334</v>
       </c>
-      <c r="L28" s="23">
+      <c r="L28" s="7">
         <v>470</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="7">
         <v>250</v>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="7">
         <v>25000</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+    <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A29" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="22">
+      <c r="B29" s="12"/>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="6">
         <v>131</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="6">
         <v>6</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="6">
         <v>14</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H29" s="6">
         <v>43</v>
       </c>
-      <c r="I29" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29" s="22">
+      <c r="I29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="6">
         <v>43</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="6">
         <v>1323</v>
       </c>
-      <c r="L29" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M29" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N29" s="22">
+      <c r="L29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="6">
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A30" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="23">
+      <c r="B30" s="12"/>
+      <c r="C30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="7">
         <v>564</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="7">
         <v>1117</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="7">
         <v>953</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="7">
         <v>413</v>
       </c>
-      <c r="H30" s="23">
+      <c r="H30" s="7">
         <v>2763</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="7">
         <v>2224</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="7">
         <v>505</v>
       </c>
-      <c r="K30" s="23">
+      <c r="K30" s="7">
         <v>23296</v>
       </c>
-      <c r="L30" s="23">
+      <c r="L30" s="7">
         <v>1000</v>
       </c>
-      <c r="M30" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="N30" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+      <c r="M30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A31" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="22">
+      <c r="B31" s="12"/>
+      <c r="C31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="6">
         <v>53</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="6">
         <v>168</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="6">
         <v>7</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="6">
         <v>16</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="6">
         <v>97</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="6">
         <v>57</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="6">
         <v>40</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="6">
         <v>1395</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="6">
         <v>517</v>
       </c>
-      <c r="M31" s="22">
+      <c r="M31" s="6">
         <v>683</v>
       </c>
-      <c r="N31" s="22">
+      <c r="N31" s="6">
         <v>507</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A32" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="23">
+      <c r="B32" s="12"/>
+      <c r="C32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="7">
         <v>50</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="7">
         <v>262</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="7">
         <v>125</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="7">
         <v>8</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="7">
         <v>1262</v>
       </c>
-      <c r="I32" s="23">
+      <c r="I32" s="7">
         <v>1187</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="7">
         <v>75</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="7">
         <v>4469</v>
       </c>
-      <c r="L32" s="23">
+      <c r="L32" s="7">
         <v>1362</v>
       </c>
-      <c r="M32" s="23">
+      <c r="M32" s="7">
         <v>2026</v>
       </c>
-      <c r="N32" s="23">
+      <c r="N32" s="7">
         <v>5747</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+    <row r="33" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A33" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="22">
+      <c r="B33" s="12"/>
+      <c r="C33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="6">
         <v>71</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="6">
         <v>234</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="6">
         <v>5</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="6">
         <v>6</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="6">
         <v>205</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I33" s="6">
         <v>173</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J33" s="6">
         <v>32</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="6">
         <v>1376</v>
       </c>
-      <c r="L33" s="22">
+      <c r="L33" s="6">
         <v>1099</v>
       </c>
-      <c r="M33" s="22">
+      <c r="M33" s="6">
         <v>1402</v>
       </c>
-      <c r="N33" s="22">
+      <c r="N33" s="6">
         <v>15266</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+    <row r="34" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A34" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="23">
+      <c r="B34" s="12"/>
+      <c r="C34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="7">
         <v>112</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="7">
         <v>456</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="7">
         <v>12</v>
       </c>
-      <c r="G34" s="23">
-        <v>19</v>
-      </c>
-      <c r="H34" s="23">
+      <c r="G34" s="7">
+        <v>19</v>
+      </c>
+      <c r="H34" s="7">
         <v>126</v>
       </c>
-      <c r="I34" s="23">
+      <c r="I34" s="7">
         <v>36</v>
       </c>
-      <c r="J34" s="23">
+      <c r="J34" s="7">
         <v>77</v>
       </c>
-      <c r="K34" s="23">
+      <c r="K34" s="7">
         <v>3141</v>
       </c>
-      <c r="L34" s="23">
+      <c r="L34" s="7">
         <v>705</v>
       </c>
-      <c r="M34" s="23">
+      <c r="M34" s="7">
         <v>1650</v>
       </c>
-      <c r="N34" s="23">
+      <c r="N34" s="7">
         <v>33872</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A35" s="20" t="s">
+    <row r="35" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A35" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="22">
+      <c r="B35" s="12"/>
+      <c r="C35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="6">
         <v>158</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="6">
         <v>393</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="6">
         <v>49</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="6">
         <v>20</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="6">
         <v>65</v>
       </c>
-      <c r="I35" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="K35" s="22">
+      <c r="I35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="6">
         <v>3607</v>
       </c>
-      <c r="L35" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N35" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="20" t="s">
+      <c r="L35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A36" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="23">
+      <c r="B36" s="12"/>
+      <c r="C36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="7">
         <v>90</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="7">
         <v>211</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="7">
         <v>12</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="7">
         <v>18</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="7">
         <v>79</v>
       </c>
-      <c r="I36" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="23">
+      <c r="I36" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="7">
         <v>79</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="7">
         <v>3619</v>
       </c>
-      <c r="L36" s="23">
+      <c r="L36" s="7">
         <v>699</v>
       </c>
-      <c r="M36" s="23">
+      <c r="M36" s="7">
         <v>1508</v>
       </c>
-      <c r="N36" s="23">
+      <c r="N36" s="7">
         <v>24818</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A37" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="22">
+      <c r="B37" s="12"/>
+      <c r="C37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="6">
         <v>89</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E37" s="6">
         <v>380</v>
       </c>
-      <c r="F37" s="22">
+      <c r="F37" s="6">
         <v>24</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="6">
         <v>21</v>
       </c>
-      <c r="H37" s="22">
+      <c r="H37" s="6">
         <v>273</v>
       </c>
-      <c r="I37" s="22">
+      <c r="I37" s="6">
         <v>188</v>
       </c>
-      <c r="J37" s="22">
+      <c r="J37" s="6">
         <v>85</v>
       </c>
-      <c r="K37" s="22">
+      <c r="K37" s="6">
         <v>3452</v>
       </c>
-      <c r="L37" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M37" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N37" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A38" s="20" t="s">
+      <c r="L37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A38" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="23">
+      <c r="B38" s="12"/>
+      <c r="C38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="7">
         <v>172</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="7">
         <v>640</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="7">
         <v>105</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="7">
         <v>39</v>
       </c>
-      <c r="H38" s="23">
+      <c r="H38" s="7">
         <v>1147</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="7">
         <v>1062</v>
       </c>
-      <c r="J38" s="23">
+      <c r="J38" s="7">
         <v>85</v>
       </c>
-      <c r="K38" s="23">
+      <c r="K38" s="7">
         <v>7586</v>
       </c>
-      <c r="L38" s="23">
+      <c r="L38" s="7">
         <v>885</v>
       </c>
-      <c r="M38" s="23">
+      <c r="M38" s="7">
         <v>466</v>
       </c>
-      <c r="N38" s="23">
+      <c r="N38" s="7">
         <v>42969</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
+    <row r="39" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A39" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="22">
+      <c r="B39" s="12"/>
+      <c r="C39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="6">
         <v>65</v>
       </c>
-      <c r="E39" s="22">
+      <c r="E39" s="6">
         <v>253</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F39" s="6">
         <v>6</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G39" s="6">
         <v>13</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="6">
         <v>132</v>
       </c>
-      <c r="I39" s="22">
+      <c r="I39" s="6">
         <v>97</v>
       </c>
-      <c r="J39" s="22">
+      <c r="J39" s="6">
         <v>42</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="6">
         <v>1603</v>
       </c>
-      <c r="L39" s="22">
+      <c r="L39" s="6">
         <v>1040</v>
       </c>
-      <c r="M39" s="22">
+      <c r="M39" s="6">
         <v>2637</v>
       </c>
-      <c r="N39" s="22">
+      <c r="N39" s="6">
         <v>38487</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A40" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="23">
+      <c r="B40" s="12"/>
+      <c r="C40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="7">
         <v>97</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="7">
         <v>205</v>
       </c>
-      <c r="F40" s="23">
-        <v>19</v>
-      </c>
-      <c r="G40" s="23">
-        <v>19</v>
-      </c>
-      <c r="H40" s="23">
+      <c r="F40" s="7">
+        <v>19</v>
+      </c>
+      <c r="G40" s="7">
+        <v>19</v>
+      </c>
+      <c r="H40" s="7">
         <v>90</v>
       </c>
-      <c r="I40" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J40" s="23">
+      <c r="I40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="7">
         <v>90</v>
       </c>
-      <c r="K40" s="23">
+      <c r="K40" s="7">
         <v>2866</v>
       </c>
-      <c r="L40" s="23">
+      <c r="L40" s="7">
         <v>1153</v>
       </c>
-      <c r="M40" s="23">
+      <c r="M40" s="7">
         <v>786</v>
       </c>
-      <c r="N40" s="23">
+      <c r="N40" s="7">
         <v>3118</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
+    <row r="41" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A41" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="22">
+      <c r="B41" s="12"/>
+      <c r="C41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="6">
         <v>175</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E41" s="6">
         <v>500</v>
       </c>
-      <c r="F41" s="22">
+      <c r="F41" s="6">
         <v>146</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="6">
         <v>39</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H41" s="6">
         <v>896</v>
       </c>
-      <c r="I41" s="22">
+      <c r="I41" s="6">
         <v>512</v>
       </c>
-      <c r="J41" s="22">
+      <c r="J41" s="6">
         <v>384</v>
       </c>
-      <c r="K41" s="22">
+      <c r="K41" s="6">
         <v>12141</v>
       </c>
-      <c r="L41" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M41" s="22">
+      <c r="L41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M41" s="6">
         <v>1000</v>
       </c>
-      <c r="N41" s="22">
+      <c r="N41" s="6">
         <v>20636</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
+    <row r="42" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A42" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="23">
+      <c r="B42" s="12"/>
+      <c r="C42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="7">
         <v>107</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="7">
         <v>590</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="7">
         <v>15</v>
       </c>
-      <c r="G42" s="23">
+      <c r="G42" s="7">
         <v>15</v>
       </c>
-      <c r="H42" s="23">
+      <c r="H42" s="7">
         <v>622</v>
       </c>
-      <c r="I42" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J42" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="K42" s="23">
+      <c r="I42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="7">
         <v>4562</v>
       </c>
-      <c r="L42" s="23">
+      <c r="L42" s="7">
         <v>805</v>
       </c>
-      <c r="M42" s="23">
+      <c r="M42" s="7">
         <v>2875</v>
       </c>
-      <c r="N42" s="23">
+      <c r="N42" s="7">
         <v>36242</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="13" x14ac:dyDescent="0.3">
-      <c r="A43" s="19" t="s">
+    <row r="43" spans="1:14" ht="13" x14ac:dyDescent="0.45">
+      <c r="A43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" s="22">
+      <c r="C43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="6">
         <v>877</v>
       </c>
-      <c r="H43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="K43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="L43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M43" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N43" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+      <c r="H43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A44" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A45" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A46" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="9" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
@@ -3046,42 +3071,17 @@
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:N3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:N4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=WILD_LIFE&amp;ShowOnWeb=true&amp;Lang=en"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=WILD_LIFE&amp;Coords=[IUCN].[TOT_KNOWN]&amp;ShowOnWeb=true&amp;Lang=en"/>
-    <hyperlink ref="A19" r:id="rId3" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=WILD_LIFE&amp;Coords=[COU].[DEU]&amp;ShowOnWeb=true&amp;Lang=en"/>
-    <hyperlink ref="A44" r:id="rId4" display="https://stats-3.oecd.org/index.aspx?DatasetCode=WILD_LIFE"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=WILD_LIFE&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=WILD_LIFE&amp;Coords=[IUCN].[TOT_KNOWN]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A19" r:id="rId3" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=WILD_LIFE&amp;Coords=[COU].[DEU]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A44" r:id="rId4" display="https://stats-3.oecd.org/index.aspx?DatasetCode=WILD_LIFE" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>